<commit_message>
Fixed: Missing data when converting from .xlsx to .html
</commit_message>
<xml_diff>
--- a/FYP Student Feedback Survey Form - Live Response .xlsx
+++ b/FYP Student Feedback Survey Form - Live Response .xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26616"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26623"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4833023-12BE-49DC-98D0-499B39F38EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{010CDEA0-14F3-4F18-A5B9-CA796E810218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>